<commit_message>
Three models are ready.
</commit_message>
<xml_diff>
--- a/MiscArtifacts/TucsonMonthlyMobility.xlsx
+++ b/MiscArtifacts/TucsonMonthlyMobility.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\My_software_develops\MobilityPyro\MobilityInference\MiscArtifacts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{784DC896-5809-4A99-9193-295E7761FD30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0470061D-FA2D-4812-9610-46F9AAD6DAB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-75" windowWidth="29040" windowHeight="15840" xr2:uid="{E5145DC8-7FF9-4C1F-B0E4-6CAAF211372E}"/>
+    <workbookView xWindow="28680" yWindow="-75" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{E5145DC8-7FF9-4C1F-B0E4-6CAAF211372E}"/>
   </bookViews>
   <sheets>
     <sheet name="Tucson" sheetId="1" r:id="rId1"/>
     <sheet name="Appleton" sheetId="2" r:id="rId2"/>
+    <sheet name="Seattle" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="33">
   <si>
     <t>2020_06</t>
   </si>
@@ -127,6 +128,15 @@
   </si>
   <si>
     <t>Using half analytical</t>
+  </si>
+  <si>
+    <t>Mobility</t>
+  </si>
+  <si>
+    <t>Multivisits</t>
+  </si>
+  <si>
+    <t>Seattle</t>
   </si>
 </sst>
 </file>
@@ -336,28 +346,52 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Tucson!$A$10:$A$16</c:f>
+              <c:f>Tucson!$A$4:$A$18</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
+                  <c:v>2020_05</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2020_06</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2020_07</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2020_08</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2020_09</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2020_10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2020_11</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2020_12</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>2021_01</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="9">
                   <c:v>2021_02</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="10">
                   <c:v>2021_03</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="11">
                   <c:v>2021_04</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="12">
                   <c:v>2021_05</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="13">
                   <c:v>2021_06</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="14">
                   <c:v>2021_07</c:v>
                 </c:pt>
               </c:strCache>
@@ -365,29 +399,53 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tucson!$B$10:$B$16</c:f>
+              <c:f>Tucson!$B$4:$B$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
+                  <c:v>955689</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1162889</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1319574</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1294644</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1389435</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1369920</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1501175</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1306806</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>1359644</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="9">
                   <c:v>1341645</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="10">
                   <c:v>1311540</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="11">
                   <c:v>1627543</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="12">
                   <c:v>1605584</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="13">
                   <c:v>1418468</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="14">
                   <c:v>1332779</c:v>
                 </c:pt>
               </c:numCache>
@@ -666,7 +724,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Tucson!$A$23:$A$39</c:f>
+              <c:f>Tucson!$A$25:$A$41</c:f>
               <c:strCache>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
@@ -725,7 +783,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tucson!$B$23:$B$39</c:f>
+              <c:f>Tucson!$B$25:$B$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="17"/>
@@ -1060,7 +1118,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Tucson!$A$10:$A$16</c:f>
+              <c:f>Tucson!$A$12:$A$18</c:f>
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
@@ -1089,7 +1147,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tucson!$C$10:$C$16</c:f>
+              <c:f>Tucson!$D$12:$D$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1138,7 +1196,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Tucson!$A$10:$A$16</c:f>
+              <c:f>Tucson!$A$12:$A$18</c:f>
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
@@ -1167,7 +1225,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tucson!$D$10:$D$16</c:f>
+              <c:f>Tucson!$E$12:$E$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1216,7 +1274,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Tucson!$A$10:$A$16</c:f>
+              <c:f>Tucson!$A$12:$A$18</c:f>
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
@@ -1245,7 +1303,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tucson!$E$10:$E$16</c:f>
+              <c:f>Tucson!$F$12:$F$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1294,7 +1352,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Tucson!$A$10:$A$16</c:f>
+              <c:f>Tucson!$A$12:$A$18</c:f>
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
@@ -1323,7 +1381,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tucson!$G$10:$G$16</c:f>
+              <c:f>Tucson!$H$12:$H$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1372,7 +1430,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Tucson!$A$10:$A$16</c:f>
+              <c:f>Tucson!$A$12:$A$18</c:f>
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
@@ -1401,7 +1459,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tucson!$H$10:$H$16</c:f>
+              <c:f>Tucson!$I$12:$I$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1419,7 +1477,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tucson!$A$10:$A$16</c:f>
+              <c:f>Tucson!$A$12:$A$18</c:f>
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
@@ -1458,7 +1516,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Tucson!$F$10:$F$16</c:f>
+              <c:f>Tucson!$G$12:$G$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1667,6 +1725,814 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1680" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Tucson multivisit</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1680" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Tucson!$A$2:$A$18</c:f>
+              <c:strCache>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>2020_03</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2020_04</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2020_05</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2020_06</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2020_07</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2020_08</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2020_09</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2020_10</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2020_11</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2020_12</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2021_01</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2021_02</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2021_03</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2021_04</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2021_05</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2021_06</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2021_07</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Tucson!$C$2:$C$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>1.684553</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.6227564999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.6836711</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.6323506999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.6182543</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.618204</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.5950120999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.5715238</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.5484743999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.5322412999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.5421644000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.533579</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.5250587</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.5376893</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.5171133999999999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.5118734</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.5158503999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A974-4DBD-962C-FC2F8F62E62A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="692795088"/>
+        <c:axId val="692796336"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="692795088"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="692796336"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="692796336"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="692795088"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1400" b="1">
+          <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+          <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Seattle!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Multivisits</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Seattle!$A$2:$A$16</c:f>
+              <c:strCache>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>2020_05</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2020_06</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2020_07</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2020_08</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2020_09</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2020_10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2020_11</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2020_12</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2021_01</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2021_02</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2021_03</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2021_04</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2021_05</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2021_06</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2021_07</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Seattle!$B$2:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>1.7511116</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.722629</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.6875066000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.6769270000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.6288369</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.6752194</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.713573</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.6747835</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.6840386000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.7237572999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.6497967</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.6656872</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.6341333</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.6316739</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.6029678999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-AB78-4559-AC3B-CF221A21C6B5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1145781023"/>
+        <c:axId val="1145781503"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1145781023"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1145781503"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1145781503"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1145781023"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1787,6 +2653,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -3296,20 +4242,1026 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>152398</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>180974</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>66674</xdr:rowOff>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>419099</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3336,16 +5288,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>4762</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>119062</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>323850</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3372,16 +5324,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>28577</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>180974</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>333377</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3403,6 +5355,85 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>476249</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{77D3AE85-30ED-49B5-8014-F6837407FF92}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>333374</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>400049</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{21F970A8-60AB-7307-A3CF-BCC80E567C34}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3708,10 +5739,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD591821-C46E-48BB-AB82-5582BC9F45EF}">
-  <dimension ref="A1:H39"/>
+  <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3719,406 +5750,476 @@
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2">
+        <v>1.684553</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3">
+        <v>1.6227564999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>14</v>
       </c>
-      <c r="B2">
+      <c r="B4">
         <v>955689</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="C4">
+        <v>1.6836711</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>0</v>
       </c>
-      <c r="B3">
+      <c r="B5">
         <v>1162889</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="C5">
+        <v>1.6323506999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>1</v>
       </c>
-      <c r="B4">
+      <c r="B6">
         <v>1319574</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="C6">
+        <v>1.6182543</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>2</v>
       </c>
-      <c r="B5">
+      <c r="B7">
         <v>1294644</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="C7">
+        <v>1.618204</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>3</v>
       </c>
-      <c r="B6">
+      <c r="B8">
         <v>1389435</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="C8">
+        <v>1.5950120999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>4</v>
       </c>
-      <c r="B7">
+      <c r="B9">
         <v>1369920</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="C9">
+        <v>1.5715238</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>5</v>
       </c>
-      <c r="B8">
+      <c r="B10">
         <v>1501175</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C10">
+        <v>1.5484743999999999</v>
+      </c>
+      <c r="D10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>6</v>
       </c>
-      <c r="B9">
+      <c r="B11">
         <v>1306806</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C11">
+        <v>1.5322412999999999</v>
+      </c>
+      <c r="D11" t="s">
         <v>29</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H11" t="s">
         <v>27</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I11" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>7</v>
       </c>
-      <c r="B10">
+      <c r="B12">
         <v>1359644</v>
       </c>
-      <c r="C10">
+      <c r="C12">
+        <v>1.5421644000000001</v>
+      </c>
+      <c r="D12">
         <v>119</v>
       </c>
-      <c r="D10">
+      <c r="E12">
         <v>381</v>
       </c>
-      <c r="E10">
+      <c r="F12">
         <v>250</v>
       </c>
-      <c r="F10">
+      <c r="G12">
         <v>618</v>
       </c>
-      <c r="G10">
+      <c r="H12">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>8</v>
       </c>
-      <c r="B11">
+      <c r="B13">
         <v>1341645</v>
       </c>
-      <c r="C11">
+      <c r="C13">
+        <v>1.533579</v>
+      </c>
+      <c r="D13">
         <v>16825</v>
       </c>
-      <c r="D11">
+      <c r="E13">
         <v>16483</v>
       </c>
-      <c r="E11">
+      <c r="F13">
         <v>16958</v>
       </c>
-      <c r="F11">
+      <c r="G13">
         <v>8445</v>
       </c>
-      <c r="G11">
+      <c r="H13">
         <v>16941</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>9</v>
       </c>
-      <c r="B12">
+      <c r="B14">
         <v>1311540</v>
       </c>
-      <c r="C12">
+      <c r="C14">
+        <v>1.5250587</v>
+      </c>
+      <c r="D14">
         <v>19090</v>
       </c>
-      <c r="D12">
+      <c r="E14">
         <v>18625</v>
       </c>
-      <c r="E12">
+      <c r="F14">
         <v>19223</v>
       </c>
-      <c r="F12">
+      <c r="G14">
         <v>11402</v>
       </c>
-      <c r="G12">
+      <c r="H14">
         <v>19206</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>10</v>
       </c>
-      <c r="B13">
+      <c r="B15">
         <v>1627543</v>
       </c>
-      <c r="C13">
+      <c r="C15">
+        <v>1.5376893</v>
+      </c>
+      <c r="D15">
         <v>53278</v>
       </c>
-      <c r="D13">
+      <c r="E15">
         <v>52948</v>
       </c>
-      <c r="E13">
+      <c r="F15">
         <v>53245</v>
       </c>
-      <c r="F13">
+      <c r="G15">
         <v>15649</v>
       </c>
-      <c r="G13">
+      <c r="H15">
         <v>53390</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>11</v>
       </c>
-      <c r="B14">
+      <c r="B16">
         <v>1605584</v>
       </c>
-      <c r="C14">
+      <c r="C16">
+        <v>1.5171133999999999</v>
+      </c>
+      <c r="D16">
         <v>56861</v>
       </c>
-      <c r="D14">
+      <c r="E16">
         <v>56531</v>
       </c>
-      <c r="E14">
+      <c r="F16">
         <v>56828</v>
       </c>
-      <c r="F14">
+      <c r="G16">
         <v>20646</v>
       </c>
-      <c r="G14">
+      <c r="H16">
         <v>56973</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>12</v>
       </c>
-      <c r="B15">
+      <c r="B17">
         <v>1418468</v>
       </c>
-      <c r="C15">
+      <c r="C17">
+        <v>1.5118734</v>
+      </c>
+      <c r="D17">
         <v>32640</v>
       </c>
-      <c r="D15">
+      <c r="E17">
         <v>32310</v>
       </c>
-      <c r="E15">
+      <c r="F17">
         <v>32607</v>
       </c>
-      <c r="F15">
+      <c r="G17">
         <v>15763</v>
       </c>
-      <c r="G15">
+      <c r="H17">
         <v>32752</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>13</v>
       </c>
-      <c r="B16">
+      <c r="B18">
         <v>1332779</v>
       </c>
-      <c r="C16">
+      <c r="C18">
+        <v>1.5158503999999999</v>
+      </c>
+      <c r="D18">
         <v>9817</v>
       </c>
-      <c r="D16">
+      <c r="E18">
         <v>9622</v>
       </c>
-      <c r="E16">
+      <c r="F18">
         <v>9729</v>
       </c>
-      <c r="F16">
+      <c r="G18">
         <v>14683</v>
       </c>
-      <c r="G16">
+      <c r="H18">
         <v>9833</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="B20" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>18</v>
       </c>
-      <c r="B23">
+      <c r="B25">
         <v>1137092284</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>17</v>
       </c>
-      <c r="B24">
+      <c r="B26">
         <v>839375816</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>14</v>
       </c>
-      <c r="B25">
+      <c r="B27">
         <v>484786181</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>0</v>
       </c>
-      <c r="B26">
+      <c r="B28">
         <v>662268483</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>1</v>
       </c>
-      <c r="B27">
+      <c r="B29">
         <v>798167696</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>2</v>
       </c>
-      <c r="B28">
+      <c r="B30">
         <v>818372346</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>3</v>
       </c>
-      <c r="B29">
+      <c r="B31">
         <v>868807672</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>4</v>
       </c>
-      <c r="B30">
+      <c r="B32">
         <v>850570021</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>5</v>
-      </c>
-      <c r="B31">
-        <v>899786594</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>6</v>
-      </c>
-      <c r="B32">
-        <v>778398948</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B33">
-        <v>817976072</v>
+        <v>899786594</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B34">
-        <v>785443403</v>
+        <v>778398948</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B35">
-        <v>747425685</v>
+        <v>817976072</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B36">
-        <v>966336263</v>
+        <v>785443403</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B37">
-        <v>970677141</v>
+        <v>747425685</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B38">
-        <v>868800299</v>
+        <v>966336263</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>11</v>
+      </c>
+      <c r="B39">
+        <v>970677141</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>12</v>
+      </c>
+      <c r="B40">
+        <v>868800299</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>13</v>
       </c>
-      <c r="B39">
+      <c r="B41">
         <v>865009560</v>
       </c>
     </row>
@@ -4134,7 +6235,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC3E1010-2E68-42C6-A37F-79C3FA41A328}">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
@@ -4382,4 +6483,148 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6458019-375C-47F0-9889-95FFAB7256E0}">
+  <dimension ref="A1:B16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2">
+        <v>1.7511116</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>1.722629</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>1.6875066000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>1.6769270000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>1.6288369</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>1.6752194</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>1.713573</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9">
+        <v>1.6747835</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10">
+        <v>1.6840386000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11">
+        <v>1.7237572999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12">
+        <v>1.6497967</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13">
+        <v>1.6656872</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14">
+        <v>1.6341333</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15">
+        <v>1.6316739</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16">
+        <v>1.6029678999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>